<commit_message>
V0 of the CRUD app
</commit_message>
<xml_diff>
--- a/Excel_files/Darna_inscription_db.xlsx
+++ b/Excel_files/Darna_inscription_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anass.harbouli\Desktop\Darna App\Excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anass.harbouli\Desktop\Darna_App\Excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB2B463-0E6D-4D7A-95AB-5739BE773C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B64BCE-2C72-409F-8F3D-22A957C69570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{91B43E86-EB18-4641-8C29-388332AFBF7C}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{91B43E86-EB18-4641-8C29-388332AFBF7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2882,9 +2882,6 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Adresse</t>
   </si>
   <si>
@@ -2894,9 +2891,6 @@
     <t>Fraterie</t>
   </si>
   <si>
-    <t>Num</t>
-  </si>
-  <si>
     <t>situation_familliale</t>
   </si>
   <si>
@@ -2915,9 +2909,6 @@
     <t>Niveau_scolaire</t>
   </si>
   <si>
-    <t>Nom et prenom</t>
-  </si>
-  <si>
     <t>Problemes_sante</t>
   </si>
   <si>
@@ -2928,6 +2919,15 @@
   </si>
   <si>
     <t>Date_naissance</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:T131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,10 +3334,10 @@
   <sheetData>
     <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>838</v>
+        <v>847</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>833</v>
@@ -3346,49 +3346,49 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>849</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>834</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>847</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>837</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>846</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>844</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>843</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>842</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>836</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>841</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>832</v>

</xml_diff>